<commit_message>
Notas da Prova 02
</commit_message>
<xml_diff>
--- a/notas.xlsx
+++ b/notas.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d53064bec2e33241/Desktop/dce540/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F1E64ED4-D701-4FF1-87FD-B580FBFE51F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="54" documentId="8_{F1E64ED4-D701-4FF1-87FD-B580FBFE51F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{79DE4631-A756-4AA6-90D5-3535B3E27E0A}"/>
   <bookViews>
     <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{0A0CDC62-7477-43D7-96EB-A35867CEC72B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -157,10 +157,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -479,8 +479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3130BEEE-6748-4784-9B13-68650E5EEC7F}">
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -489,41 +489,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -535,6 +535,10 @@
         <f>12+20+10+6+15+10</f>
         <v>73</v>
       </c>
+      <c r="C7">
+        <f>10+5+15+15+25+10</f>
+        <v>80</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -544,6 +548,10 @@
         <f>15+19+10+4+18+10</f>
         <v>76</v>
       </c>
+      <c r="C8">
+        <f>10+0+13+10+12+10</f>
+        <v>55</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -552,6 +560,9 @@
       <c r="B9">
         <v>0</v>
       </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -560,6 +571,10 @@
       <c r="B10">
         <v>0</v>
       </c>
+      <c r="C10">
+        <f>10+0+15+20+27+10</f>
+        <v>82</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -569,6 +584,9 @@
         <f>12+7+5+8+5+0</f>
         <v>37</v>
       </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -578,6 +596,10 @@
         <f>15+14+10+10+15+0</f>
         <v>64</v>
       </c>
+      <c r="C12">
+        <f>9+10+10+18+27+10</f>
+        <v>84</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -587,6 +609,10 @@
         <f>15+18+10+10+16+0</f>
         <v>69</v>
       </c>
+      <c r="C13">
+        <f>10+0+15+18+25+10</f>
+        <v>78</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -596,6 +622,10 @@
         <f>13+20+5+10+15+10</f>
         <v>73</v>
       </c>
+      <c r="C14">
+        <f>10+6+12+20+20+5</f>
+        <v>73</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -605,6 +635,10 @@
         <f>15+18+9+10+15+10</f>
         <v>77</v>
       </c>
+      <c r="C15">
+        <f>9+0+13+12+18+5</f>
+        <v>57</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -614,8 +648,12 @@
         <f>15+18+9+10+15+10</f>
         <v>77</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C16">
+        <f>6+6+14+20+30+10</f>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -623,8 +661,12 @@
         <f>14+20+10+10+20+10</f>
         <v>84</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C17">
+        <f>8+0+12+16+27+10</f>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -632,8 +674,12 @@
         <f>15+20+10+10+20+10</f>
         <v>85</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C18">
+        <f>10+10+15+20+27+10</f>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -641,16 +687,23 @@
         <f>15+20+10+10+20+10</f>
         <v>85</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C19">
+        <f>9+7+15+20+30+10</f>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>12</v>
       </c>
       <c r="B20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>13</v>
       </c>
@@ -658,8 +711,12 @@
         <f>15+20+10+10+20+10</f>
         <v>85</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C21">
+        <f>10+3+15+18+20+10</f>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -667,8 +724,12 @@
         <f>15+20+10+10+20+10</f>
         <v>85</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C22">
+        <f>10+5+15+16+22+10</f>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -676,16 +737,23 @@
         <f>15+20+10+10+20+5</f>
         <v>80</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C23">
+        <f>10+6+15+16+30+10</f>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>25</v>
       </c>
       <c r="B24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -693,8 +761,12 @@
         <f>15+20+10+10+20+15</f>
         <v>90</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C25">
+        <f>8+14+15+16+28+10</f>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -702,8 +774,12 @@
         <f>15+20+10+10+20+10</f>
         <v>85</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C26">
+        <f>10+6+15+16+28+8</f>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>14</v>
       </c>
@@ -711,8 +787,12 @@
         <f>15+20+10+10+20+10</f>
         <v>85</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C27">
+        <f>10+0+12+10+25+10</f>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>15</v>
       </c>
@@ -720,8 +800,12 @@
         <f>15+20+10+10+15+10</f>
         <v>80</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C28">
+        <f>10+5+15+15+20+8</f>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -729,14 +813,22 @@
         <f>15+18+9+10+15+10</f>
         <v>77</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C29">
+        <f>10+0+15+15+20+6</f>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>16</v>
       </c>
       <c r="B30">
         <f>15+20+10+10+15+10</f>
         <v>80</v>
+      </c>
+      <c r="C30">
+        <f>10+5+12+15+30+10</f>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Notas da prova 03
</commit_message>
<xml_diff>
--- a/notas.xlsx
+++ b/notas.xlsx
@@ -1,31 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d53064bec2e33241/Desktop/dce540/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="54" documentId="8_{F1E64ED4-D701-4FF1-87FD-B580FBFE51F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{79DE4631-A756-4AA6-90D5-3535B3E27E0A}"/>
+  <xr:revisionPtr revIDLastSave="87" documentId="8_{F1E64ED4-D701-4FF1-87FD-B580FBFE51F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BFBAA892-32ED-4A27-9854-265F6D9404B6}"/>
   <bookViews>
     <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{0A0CDC62-7477-43D7-96EB-A35867CEC72B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>As notas das provas variam entre 0 e 100</t>
   </si>
@@ -112,6 +119,9 @@
   </si>
   <si>
     <t>2018.1.08.023</t>
+  </si>
+  <si>
+    <t>Prova 03</t>
   </si>
 </sst>
 </file>
@@ -480,7 +490,7 @@
   <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -526,6 +536,9 @@
       <c r="C6" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="D6" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -539,6 +552,10 @@
         <f>10+5+15+15+25+10</f>
         <v>80</v>
       </c>
+      <c r="D7">
+        <f>15+15+15+20+15+15</f>
+        <v>95</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -552,6 +569,10 @@
         <f>10+0+13+10+12+10</f>
         <v>55</v>
       </c>
+      <c r="D8">
+        <f>10+15+0+20+9+10</f>
+        <v>64</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -563,6 +584,9 @@
       <c r="C9">
         <v>0</v>
       </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -575,6 +599,10 @@
         <f>10+0+15+20+27+10</f>
         <v>82</v>
       </c>
+      <c r="D10">
+        <f>3+10+15+20+12+0</f>
+        <v>60</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -587,6 +615,9 @@
       <c r="C11">
         <v>0</v>
       </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -600,6 +631,10 @@
         <f>9+10+10+18+27+10</f>
         <v>84</v>
       </c>
+      <c r="D12">
+        <f>15+15+15+0+15+15</f>
+        <v>75</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -613,6 +648,10 @@
         <f>10+0+15+18+25+10</f>
         <v>78</v>
       </c>
+      <c r="D13">
+        <f>10+15+15+20+15+20</f>
+        <v>95</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -626,6 +665,10 @@
         <f>10+6+12+20+20+5</f>
         <v>73</v>
       </c>
+      <c r="D14">
+        <f>15+15+15+20+15+15</f>
+        <v>95</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -639,6 +682,10 @@
         <f>9+0+13+12+18+5</f>
         <v>57</v>
       </c>
+      <c r="D15">
+        <f>15+10+15+20+12+0</f>
+        <v>72</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -652,8 +699,12 @@
         <f>6+6+14+20+30+10</f>
         <v>86</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D16">
+        <f>15+15+15+20+15+12</f>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -665,8 +716,12 @@
         <f>8+0+12+16+27+10</f>
         <v>73</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D17">
+        <f>15+5+15+20+12+15</f>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -678,8 +733,11 @@
         <f>10+10+15+20+27+10</f>
         <v>92</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D18">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -691,8 +749,11 @@
         <f>9+7+15+20+30+10</f>
         <v>91</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D19">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -702,8 +763,11 @@
       <c r="C20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>13</v>
       </c>
@@ -715,8 +779,12 @@
         <f>10+3+15+18+20+10</f>
         <v>76</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D21">
+        <f>15+15+15+20+15+18</f>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -728,8 +796,12 @@
         <f>10+5+15+16+22+10</f>
         <v>78</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D22">
+        <f>15+15+15+20+15+15</f>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -741,8 +813,12 @@
         <f>10+6+15+16+30+10</f>
         <v>87</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D23">
+        <f>15+15+15+20+15+15</f>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -752,8 +828,11 @@
       <c r="C24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -765,8 +844,12 @@
         <f>8+14+15+16+28+10</f>
         <v>91</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D25">
+        <f>8+12+15+20+12+15</f>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -778,8 +861,12 @@
         <f>10+6+15+16+28+8</f>
         <v>83</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D26">
+        <f>15+15+15+20+15+15</f>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>14</v>
       </c>
@@ -791,8 +878,12 @@
         <f>10+0+12+10+25+10</f>
         <v>67</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D27">
+        <f>15+15+15+20+15+10</f>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>15</v>
       </c>
@@ -804,8 +895,12 @@
         <f>10+5+15+15+20+8</f>
         <v>73</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D28">
+        <f>15+15+15+20+15+10</f>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -817,8 +912,12 @@
         <f>10+0+15+15+20+6</f>
         <v>66</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D29">
+        <f>15+12+15+20+12+12</f>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>16</v>
       </c>
@@ -829,6 +928,10 @@
       <c r="C30">
         <f>10+5+12+15+30+10</f>
         <v>82</v>
+      </c>
+      <c r="D30">
+        <f>15+15+15+20+15+15</f>
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Troca da primeira com a segunda linha da tabela (ordem alfabética estava errada)
</commit_message>
<xml_diff>
--- a/notas.xlsx
+++ b/notas.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iagoa\OneDrive\Desktop\dce540\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1C16FCF0-D8DB-4AAA-AB38-ADAC8E346543}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F6F4985-48FE-4A74-A9E5-BA15CBF1873A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{FEA59ED9-6309-4FD7-BAB7-52937329DDA7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -134,7 +134,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -146,6 +146,12 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -183,7 +189,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -193,6 +199,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -509,7 +519,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4E1061E-5799-46BC-9C1D-4FD1F59D576D}">
-  <dimension ref="A4:D32"/>
+  <dimension ref="A4:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B1" sqref="B1:B1048576"/>
@@ -520,7 +530,7 @@
     <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -534,28 +544,27 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="2">
-        <f>15+20+9+14+20+7</f>
-        <v>85</v>
+        <v>23</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>2</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="B6" s="4">
+        <v>85</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -566,7 +575,7 @@
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>4</v>
       </c>
@@ -576,8 +585,9 @@
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="J8" s="2"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -587,8 +597,11 @@
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="6"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>24</v>
       </c>
@@ -599,7 +612,7 @@
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -610,7 +623,7 @@
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>6</v>
       </c>
@@ -621,7 +634,7 @@
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -631,7 +644,7 @@
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>8</v>
       </c>
@@ -642,7 +655,7 @@
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -653,7 +666,7 @@
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
Atualização da nota de 2017.1.08.044
</commit_message>
<xml_diff>
--- a/notas.xlsx
+++ b/notas.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iagoa\OneDrive\Desktop\dce540\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F6F4985-48FE-4A74-A9E5-BA15CBF1873A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{362D208F-2618-4BF6-A4C2-F24EE4977D2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{FEA59ED9-6309-4FD7-BAB7-52937329DDA7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,6 +25,7 @@
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -521,8 +522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4E1061E-5799-46BC-9C1D-4FD1F59D576D}">
   <dimension ref="A4:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B13" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -726,8 +727,8 @@
         <v>13</v>
       </c>
       <c r="B21" s="2">
-        <f>15+17+10+15+20+7</f>
-        <v>84</v>
+        <f>15+17+10+15+20+14</f>
+        <v>91</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>

</xml_diff>

<commit_message>
Notas finais da disciplina
</commit_message>
<xml_diff>
--- a/notas.xlsx
+++ b/notas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iagoa\OneDrive\Desktop\dce540\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8A8870F-B8D1-4A90-B380-FC45E1C214D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2635DD1A-EC60-4C8C-BE65-873BCDBEB9BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{FEA59ED9-6309-4FD7-BAB7-52937329DDA7}"/>
   </bookViews>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Matrícula</t>
   </si>
@@ -75,9 +75,6 @@
     <t>2017.1.08.036</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>2019.1.08.042</t>
   </si>
   <si>
@@ -163,6 +160,18 @@
   </si>
   <si>
     <t>2014.1.08.034</t>
+  </si>
+  <si>
+    <t>Exercício 01</t>
+  </si>
+  <si>
+    <t>Exercício 02</t>
+  </si>
+  <si>
+    <t>Nota final</t>
+  </si>
+  <si>
+    <t>Média</t>
   </si>
 </sst>
 </file>
@@ -237,7 +246,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -251,6 +260,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -570,12 +582,14 @@
   <dimension ref="A4:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -583,27 +597,53 @@
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>22</v>
+      <c r="E4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>2</v>
+        <v>22</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2">
+        <f t="shared" ref="G5:G6" si="0">AVERAGE(E5:F5)</f>
+        <v>0</v>
+      </c>
+      <c r="H5" s="7">
+        <f>(0.3*B5+0.3*C5+0.3*D5+0.05*E5+0.05*F5)/10</f>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -621,10 +661,24 @@
         <f>12+7+15+7+6+20</f>
         <v>67</v>
       </c>
+      <c r="E6" s="4">
+        <v>0</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H6" s="7">
+        <f>(0.3*B6+0.3*C6+0.3*D6+0.05*E6+0.05*F6)/10</f>
+        <v>6.8699999999999992</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B7" s="2">
         <f>15+13+10+13+20+14</f>
@@ -638,10 +692,24 @@
         <f>15+18+15+12+15+20</f>
         <v>95</v>
       </c>
+      <c r="E7" s="2">
+        <v>100</v>
+      </c>
+      <c r="F7" s="2">
+        <v>90</v>
+      </c>
+      <c r="G7" s="2">
+        <f>AVERAGE(E7:F7)</f>
+        <v>95</v>
+      </c>
+      <c r="H7" s="7">
+        <f t="shared" ref="H7:H31" si="1">(0.3*B7+0.3*C7+0.3*D7+0.05*E7+0.05*F7)/10</f>
+        <v>8.870000000000001</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B8" s="4">
         <f>15+17+10+15+20+14</f>
@@ -655,11 +723,25 @@
         <f>15+20+15+15+15+20</f>
         <v>100</v>
       </c>
+      <c r="E8" s="4">
+        <v>100</v>
+      </c>
+      <c r="F8" s="4">
+        <v>100</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" ref="G8:G31" si="2">AVERAGE(E8:F8)</f>
+        <v>100</v>
+      </c>
+      <c r="H8" s="7">
+        <f t="shared" si="1"/>
+        <v>9.49</v>
+      </c>
       <c r="J8" s="2"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9" s="2">
         <f>15+19+8+15+20+7</f>
@@ -673,13 +755,26 @@
         <f>15+13+15+8+7+16</f>
         <v>74</v>
       </c>
-      <c r="H9" s="5"/>
+      <c r="E9" s="2">
+        <v>0</v>
+      </c>
+      <c r="F9" s="2">
+        <v>100</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="H9" s="7">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
       <c r="I9" s="5"/>
       <c r="J9" s="6"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B10" s="4">
         <f>15+18+4+14+20+7</f>
@@ -693,10 +788,24 @@
         <f>12+15+8+8+15+20</f>
         <v>78</v>
       </c>
+      <c r="E10" s="4">
+        <v>0</v>
+      </c>
+      <c r="F10" s="4">
+        <v>50</v>
+      </c>
+      <c r="G10" s="2">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="H10" s="7">
+        <f t="shared" si="1"/>
+        <v>7.18</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11" s="2">
         <f>15+18+9+13+20+7</f>
@@ -710,10 +819,24 @@
         <f>14+15+15+7+15+20</f>
         <v>86</v>
       </c>
+      <c r="E11" s="2">
+        <v>75</v>
+      </c>
+      <c r="F11" s="2">
+        <v>100</v>
+      </c>
+      <c r="G11" s="2">
+        <f t="shared" si="2"/>
+        <v>87.5</v>
+      </c>
+      <c r="H11" s="7">
+        <f t="shared" si="1"/>
+        <v>8.4049999999999994</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B12" s="4">
         <f>15+14+4+10+20+20</f>
@@ -727,24 +850,52 @@
         <f>15+15+15+15+12+20</f>
         <v>92</v>
       </c>
+      <c r="E12" s="4">
+        <v>100</v>
+      </c>
+      <c r="F12" s="4">
+        <v>0</v>
+      </c>
+      <c r="G12" s="2">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="H12" s="7">
+        <f t="shared" si="1"/>
+        <v>7.7899999999999991</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>2</v>
+        <v>6</v>
+      </c>
+      <c r="B13" s="2">
+        <v>0</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0</v>
+      </c>
+      <c r="F13" s="2">
+        <v>0</v>
+      </c>
+      <c r="G13" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H13" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B14" s="4">
         <f>15+20+8+15+20+14</f>
@@ -758,10 +909,24 @@
         <f>14+20+15+15+15+20</f>
         <v>99</v>
       </c>
+      <c r="E14" s="4">
+        <v>100</v>
+      </c>
+      <c r="F14" s="4">
+        <v>95</v>
+      </c>
+      <c r="G14" s="2">
+        <f t="shared" si="2"/>
+        <v>97.5</v>
+      </c>
+      <c r="H14" s="7">
+        <f t="shared" si="1"/>
+        <v>8.9250000000000007</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B15" s="2">
         <f>15+15+7+13+20+7</f>
@@ -775,10 +940,24 @@
         <f>3+12+12+7+5+12</f>
         <v>51</v>
       </c>
+      <c r="E15" s="2">
+        <v>0</v>
+      </c>
+      <c r="F15" s="2">
+        <v>0</v>
+      </c>
+      <c r="G15" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H15" s="7">
+        <f t="shared" si="1"/>
+        <v>6.2399999999999993</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B16" s="4">
         <f>15+17+9+11+16+14</f>
@@ -792,10 +971,24 @@
         <f>8+10+10+10+7+20</f>
         <v>65</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E16" s="4">
+        <v>100</v>
+      </c>
+      <c r="F16" s="4">
+        <v>95</v>
+      </c>
+      <c r="G16" s="2">
+        <f t="shared" si="2"/>
+        <v>97.5</v>
+      </c>
+      <c r="H16" s="7">
+        <f t="shared" si="1"/>
+        <v>7.6949999999999985</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B17" s="2">
         <f>15+16+8+9+20+7</f>
@@ -809,10 +1002,24 @@
         <f>10+15+12+12+7+18</f>
         <v>74</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E17" s="2">
+        <v>100</v>
+      </c>
+      <c r="F17" s="2">
+        <v>95</v>
+      </c>
+      <c r="G17" s="2">
+        <f t="shared" si="2"/>
+        <v>97.5</v>
+      </c>
+      <c r="H17" s="7">
+        <f t="shared" si="1"/>
+        <v>7.875</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B18" s="4">
         <f>15+20+10+15+20+20</f>
@@ -826,10 +1033,24 @@
         <f>15+20+15+15+15+20</f>
         <v>100</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E18" s="4">
+        <v>100</v>
+      </c>
+      <c r="F18" s="4">
+        <v>95</v>
+      </c>
+      <c r="G18" s="2">
+        <f t="shared" si="2"/>
+        <v>97.5</v>
+      </c>
+      <c r="H18" s="7">
+        <f t="shared" si="1"/>
+        <v>9.6750000000000007</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B19" s="2">
         <f>15+12+8+13+20+7</f>
@@ -843,10 +1064,24 @@
         <f>10+15+15+15+15+20</f>
         <v>90</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E19" s="2">
+        <v>100</v>
+      </c>
+      <c r="F19" s="2">
+        <v>95</v>
+      </c>
+      <c r="G19" s="2">
+        <f t="shared" si="2"/>
+        <v>97.5</v>
+      </c>
+      <c r="H19" s="7">
+        <f t="shared" si="1"/>
+        <v>8.5650000000000013</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B20" s="4">
         <f>15+18+7+13+20+14</f>
@@ -860,10 +1095,24 @@
         <f>15+15+15+15+12+20</f>
         <v>92</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E20" s="4">
+        <v>100</v>
+      </c>
+      <c r="F20" s="4">
+        <v>0</v>
+      </c>
+      <c r="G20" s="2">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="H20" s="7">
+        <f t="shared" si="1"/>
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B21" s="2">
         <f>15+17+10+15+20+14</f>
@@ -877,10 +1126,24 @@
         <f>15+15+15+12+14+20</f>
         <v>91</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E21" s="2">
+        <v>100</v>
+      </c>
+      <c r="F21" s="2">
+        <v>100</v>
+      </c>
+      <c r="G21" s="2">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="H21" s="7">
+        <f t="shared" si="1"/>
+        <v>8.86</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B22" s="4">
         <f>15+20+10+15+20+7</f>
@@ -894,10 +1157,24 @@
         <f>15+20+15+15+15+20</f>
         <v>100</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E22" s="4">
+        <v>100</v>
+      </c>
+      <c r="F22" s="4">
+        <v>100</v>
+      </c>
+      <c r="G22" s="2">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="H22" s="7">
+        <f t="shared" si="1"/>
+        <v>9.16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B23" s="2">
         <f>15+18+7+15+20+7</f>
@@ -911,25 +1188,53 @@
         <f>10+20+15+15+12+20</f>
         <v>92</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E23" s="2">
+        <v>0</v>
+      </c>
+      <c r="F23" s="2">
+        <v>50</v>
+      </c>
+      <c r="G23" s="2">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="H23" s="7">
+        <f t="shared" si="1"/>
+        <v>7.8699999999999992</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>2</v>
+        <v>27</v>
+      </c>
+      <c r="B24" s="4">
+        <v>0</v>
       </c>
       <c r="C24" s="4">
         <f>2+10+20+10+5+0</f>
         <v>47</v>
       </c>
-      <c r="D24" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D24" s="4">
+        <v>0</v>
+      </c>
+      <c r="E24" s="4">
+        <v>0</v>
+      </c>
+      <c r="F24" s="4">
+        <v>0</v>
+      </c>
+      <c r="G24" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H24" s="7">
+        <f t="shared" si="1"/>
+        <v>1.41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B25" s="2">
         <f>15+14+10+15+20+14</f>
@@ -943,10 +1248,24 @@
         <f>15+20+15+7+15+20</f>
         <v>92</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E25" s="2">
+        <v>100</v>
+      </c>
+      <c r="F25" s="2">
+        <v>90</v>
+      </c>
+      <c r="G25" s="2">
+        <f t="shared" si="2"/>
+        <v>95</v>
+      </c>
+      <c r="H25" s="7">
+        <f t="shared" si="1"/>
+        <v>8.9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B26" s="4">
         <f>15+18+9+14+20+7</f>
@@ -960,10 +1279,24 @@
         <f>15+15+15+15+15+20</f>
         <v>95</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E26" s="4">
+        <v>0</v>
+      </c>
+      <c r="F26" s="4">
+        <v>100</v>
+      </c>
+      <c r="G26" s="2">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="H26" s="7">
+        <f t="shared" si="1"/>
+        <v>8.0299999999999994</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B27" s="2">
         <f>15+20+10+15+20+14</f>
@@ -977,10 +1310,24 @@
         <f>15+20+15+15+15+20</f>
         <v>100</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E27" s="2">
+        <v>0</v>
+      </c>
+      <c r="F27" s="2">
+        <v>95</v>
+      </c>
+      <c r="G27" s="2">
+        <f t="shared" si="2"/>
+        <v>47.5</v>
+      </c>
+      <c r="H27" s="7">
+        <f t="shared" si="1"/>
+        <v>8.6950000000000003</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B28" s="4">
         <f>12+16+10+15+20+14</f>
@@ -994,10 +1341,24 @@
         <f>14+20+15+15+15+20</f>
         <v>99</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E28" s="4">
+        <v>100</v>
+      </c>
+      <c r="F28" s="4">
+        <v>95</v>
+      </c>
+      <c r="G28" s="2">
+        <f t="shared" si="2"/>
+        <v>97.5</v>
+      </c>
+      <c r="H28" s="7">
+        <f t="shared" si="1"/>
+        <v>9.254999999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B29" s="2">
         <f>15+15+8+15+20+14</f>
@@ -1011,10 +1372,24 @@
         <f>8+15+12+15+12+20</f>
         <v>82</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E29" s="2">
+        <v>75</v>
+      </c>
+      <c r="F29" s="2">
+        <v>95</v>
+      </c>
+      <c r="G29" s="2">
+        <f t="shared" si="2"/>
+        <v>85</v>
+      </c>
+      <c r="H29" s="7">
+        <f t="shared" si="1"/>
+        <v>8.5599999999999987</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B30" s="4">
         <f>15+16+10+15+20+14</f>
@@ -1028,10 +1403,24 @@
         <f>15+20+15+15+15+20</f>
         <v>100</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E30" s="4">
+        <v>0</v>
+      </c>
+      <c r="F30" s="4">
+        <v>0</v>
+      </c>
+      <c r="G30" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H30" s="7">
+        <f t="shared" si="1"/>
+        <v>8.1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B31" s="2">
         <f>15+20+9+14+20+7</f>
@@ -1045,8 +1434,22 @@
         <f>15+10+12+12+0+20</f>
         <v>69</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E31" s="2">
+        <v>100</v>
+      </c>
+      <c r="F31" s="2">
+        <v>95</v>
+      </c>
+      <c r="G31" s="2">
+        <f t="shared" si="2"/>
+        <v>97.5</v>
+      </c>
+      <c r="H31" s="7">
+        <f t="shared" si="1"/>
+        <v>7.9950000000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>

</xml_diff>